<commit_message>
Upgraded px_log_fs to mark oldest records as archived. Not backwards compatible with existing file system!
</commit_message>
<xml_diff>
--- a/doc/images/log_fs/log_fs.xlsx
+++ b/doc/images/log_fs/log_fs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\PICONOMIX\libraries\piconomix-fwlib\trunk\doc\images\log_fs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\PICONOMIX\libraries\piconomix-fwlib\doc\images\log_fs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECD947A-4023-4B2E-81F9-3A45D3A99084}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61B94F4-498D-42A2-94AF-D6DE16DD5F04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Key" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>F</t>
   </si>
@@ -93,21 +93,9 @@
     <t>USED</t>
   </si>
   <si>
-    <t>0x5A</t>
-  </si>
-  <si>
-    <t>0101_1010b</t>
-  </si>
-  <si>
     <t>1111_1111b</t>
   </si>
   <si>
-    <t>0xA5</t>
-  </si>
-  <si>
-    <t>0001_1111b</t>
-  </si>
-  <si>
     <t>0000_0000b</t>
   </si>
   <si>
@@ -139,6 +127,36 @@
   </si>
   <si>
     <t>7. LAST is at page 6 and FIRST is at page 7 (largest diff = 85)</t>
+  </si>
+  <si>
+    <t>0x55</t>
+  </si>
+  <si>
+    <t>0101_1111b</t>
+  </si>
+  <si>
+    <t>USED+A</t>
+  </si>
+  <si>
+    <t>0101_0101b</t>
+  </si>
+  <si>
+    <t>RECORD+A</t>
+  </si>
+  <si>
+    <t>0xAA</t>
+  </si>
+  <si>
+    <t>0xAF</t>
+  </si>
+  <si>
+    <t>0x5F</t>
+  </si>
+  <si>
+    <t>1010_1111b</t>
+  </si>
+  <si>
+    <t>1010_1010b</t>
   </si>
 </sst>
 </file>
@@ -170,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,6 +240,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -421,6 +451,10 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -814,7 +848,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H3" s="20"/>
     </row>
@@ -827,58 +861,90 @@
         <v>22</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="20"/>
-      <c r="C5" s="25" t="s">
-        <v>2</v>
+      <c r="C5" s="30" t="s">
+        <v>21</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="20"/>
-      <c r="C6" s="6" t="s">
-        <v>3</v>
+      <c r="C6" s="25" t="s">
+        <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="20"/>
+      <c r="C7" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
+      <c r="C8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="H8" s="20"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
+      <c r="H9" s="20"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -910,7 +976,7 @@
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2" s="8"/>
       <c r="C2" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -1068,7 +1134,7 @@
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
       <c r="C7" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -1226,7 +1292,7 @@
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -1420,7 +1486,7 @@
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
       <c r="C17" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -1614,7 +1680,7 @@
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B22" s="8"/>
       <c r="C22" s="9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -1812,7 +1878,7 @@
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B27" s="8"/>
       <c r="C27" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -2010,7 +2076,7 @@
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B32" s="8"/>
       <c r="C32" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -2230,7 +2296,7 @@
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="8"/>
       <c r="C3" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2245,10 +2311,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Changed page marker names to PAGE and PAGE_A to clarify meaning
</commit_message>
<xml_diff>
--- a/doc/images/log_fs/log_fs.xlsx
+++ b/doc/images/log_fs/log_fs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\PICONOMIX\libraries\piconomix-fwlib\doc\images\log_fs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archive\Work\PICONOMIX\libraries\piconomix-fwlib\doc\images\log_fs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61B94F4-498D-42A2-94AF-D6DE16DD5F04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115FB1A9-C03A-48CE-A765-AE00A5BDC156}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>F</t>
   </si>
@@ -87,12 +87,6 @@
     <t>n+2</t>
   </si>
   <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>USED</t>
-  </si>
-  <si>
     <t>1111_1111b</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>0101_1111b</t>
   </si>
   <si>
-    <t>USED+A</t>
-  </si>
-  <si>
     <t>0101_0101b</t>
   </si>
   <si>
@@ -157,6 +148,21 @@
   </si>
   <si>
     <t>1010_1010b</t>
+  </si>
+  <si>
+    <t>PAGE</t>
+  </si>
+  <si>
+    <t>PAGE+A</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>P*</t>
+  </si>
+  <si>
+    <t>R*</t>
   </si>
 </sst>
 </file>
@@ -848,39 +854,39 @@
         <v>5</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="20"/>
       <c r="C4" s="26" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="20"/>
       <c r="C5" s="30" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="H5" s="20"/>
     </row>
@@ -893,26 +899,26 @@
         <v>7</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="20"/>
       <c r="C7" s="31" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H7" s="20"/>
     </row>
@@ -928,7 +934,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H8" s="20"/>
     </row>
@@ -976,7 +982,7 @@
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2" s="8"/>
       <c r="C2" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -1134,7 +1140,7 @@
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
       <c r="C7" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -1292,7 +1298,7 @@
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
       <c r="C12" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -1486,7 +1492,7 @@
     <row r="17" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
       <c r="C17" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -1680,7 +1686,7 @@
     <row r="22" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B22" s="8"/>
       <c r="C22" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -1878,7 +1884,7 @@
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B27" s="8"/>
       <c r="C27" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -2076,7 +2082,7 @@
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B32" s="8"/>
       <c r="C32" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -2296,7 +2302,7 @@
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="8"/>
       <c r="C3" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -2311,10 +2317,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>13</v>

</xml_diff>